<commit_message>
Attendance for 6th March
</commit_message>
<xml_diff>
--- a/Attendance Tracker.xlsx
+++ b/Attendance Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oneibm4\Desktop\group-project-25-1-the-anti-statics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317FA7B8-ED46-44FA-BB08-800B5878EF2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE03F2B-CAD9-49D4-8D9F-FEB79507D0CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -398,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F67"/>
+  <dimension ref="A2:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,16 +454,16 @@
         <v>0</v>
       </c>
       <c r="C4" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -474,16 +474,16 @@
         <v>0</v>
       </c>
       <c r="C5" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -508,27 +508,27 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>45720</v>
+        <v>45722</v>
       </c>
       <c r="B7" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D7" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>45721</v>
+        <v>45723</v>
       </c>
       <c r="B8" s="3" t="b">
         <v>0</v>
@@ -547,9 +547,6 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>45722</v>
-      </c>
       <c r="B9" s="3" t="b">
         <v>0</v>
       </c>
@@ -567,9 +564,6 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>45723</v>
-      </c>
       <c r="B10" s="3" t="b">
         <v>0</v>
       </c>
@@ -1518,40 +1512,6 @@
         <v>0</v>
       </c>
       <c r="F65" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B66" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C66" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D66" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F66" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B67" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C67" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D67" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F67" s="3" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Attendance for 7th March
</commit_message>
<xml_diff>
--- a/Attendance Tracker.xlsx
+++ b/Attendance Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oneibm4\Desktop\group-project-25-1-the-anti-statics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE03F2B-CAD9-49D4-8D9F-FEB79507D0CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56CE483-6E6F-47C1-A05D-48C40CDEE248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3570" yWindow="1065" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
   <dimension ref="A2:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,19 +531,19 @@
         <v>45723</v>
       </c>
       <c r="B8" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>